<commit_message>
complete new customer and new account
</commit_message>
<xml_diff>
--- a/src/main/resources/customer-testcase.xlsx
+++ b/src/main/resources/customer-testcase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chicken/source/assignment/ki2nam3/tester/selenium/demo/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C763D8-BCDC-494B-8D9E-DC13DF1EF63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{78F3D963-5506-824B-82D3-F3B15B092EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14660" yWindow="3200" windowWidth="27640" windowHeight="16940" xr2:uid="{7AC8D51E-096D-E24F-97A6-0600BE4379BD}"/>
+    <workbookView xWindow="10760" yWindow="3200" windowWidth="27640" windowHeight="16940" xr2:uid="{7AC8D51E-096D-E24F-97A6-0600BE4379BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="43">
   <si>
     <t>male</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>01/10/2014</t>
+  </si>
+  <si>
+    <t>abcdef123456@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -547,7 +550,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,7 +586,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="J1" t="s">
         <v>6</v>
@@ -1150,24 +1153,24 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I1" r:id="rId1" xr:uid="{FC75257A-4F68-CC47-9B70-59276089ED63}"/>
-    <hyperlink ref="I2" r:id="rId2" xr:uid="{F2BDB99D-0024-1147-A670-F95AAD69C480}"/>
-    <hyperlink ref="I3" r:id="rId3" xr:uid="{BFDCB0FE-A315-3B4B-B129-68FCC56456D3}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{CA7B26A6-EC00-504B-85FF-759EC47D3524}"/>
-    <hyperlink ref="I6" r:id="rId5" display="mailto:abcd1234@gmail.com" xr:uid="{9807E65A-EFD7-4A45-975C-3BEBCEC18E69}"/>
-    <hyperlink ref="I4" r:id="rId6" xr:uid="{2C794336-F302-BF40-A6A8-F6430B6F5C8D}"/>
-    <hyperlink ref="I7" r:id="rId7" display="mailto:abcd1234@gmail.com" xr:uid="{1B7261E4-5300-5243-947E-BD3D9CAB8CE1}"/>
-    <hyperlink ref="I8" r:id="rId8" xr:uid="{DE7252F2-5BE8-CA4D-844C-508F345F69CD}"/>
-    <hyperlink ref="I9" r:id="rId9" xr:uid="{5495C219-2B02-C24B-848A-9BD92DACAC86}"/>
-    <hyperlink ref="I10" r:id="rId10" xr:uid="{D8835B11-7EE3-8245-AA5D-21C0D0311A7E}"/>
-    <hyperlink ref="I11" r:id="rId11" xr:uid="{83F21545-BDEF-DD48-9EFC-DA5824554D7D}"/>
-    <hyperlink ref="I12" r:id="rId12" xr:uid="{047DC6A4-66F6-F44C-9601-E12B7266B99C}"/>
-    <hyperlink ref="I13" r:id="rId13" xr:uid="{3B24F876-C054-B649-8B13-844E0898208C}"/>
-    <hyperlink ref="I14" r:id="rId14" xr:uid="{AE984405-5C38-B842-A2EC-FC6B17AAFD6C}"/>
-    <hyperlink ref="I15" r:id="rId15" display="abcd1234@gmail.com" xr:uid="{A9D42DA4-D802-0546-BA7B-31323FAA663B}"/>
-    <hyperlink ref="I16" r:id="rId16" display="abcd1234@gmail.com" xr:uid="{BBBD71DE-D4EF-F442-A4B2-BF9E5039F614}"/>
-    <hyperlink ref="I18" r:id="rId17" xr:uid="{FA25E08F-EB37-2B4C-B827-7B0F396795F4}"/>
-    <hyperlink ref="I19" r:id="rId18" xr:uid="{AE4E9F05-45A6-2342-9262-7AD7E240528D}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{F2BDB99D-0024-1147-A670-F95AAD69C480}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{BFDCB0FE-A315-3B4B-B129-68FCC56456D3}"/>
+    <hyperlink ref="I5" r:id="rId3" xr:uid="{CA7B26A6-EC00-504B-85FF-759EC47D3524}"/>
+    <hyperlink ref="I6" r:id="rId4" display="mailto:abcd1234@gmail.com" xr:uid="{9807E65A-EFD7-4A45-975C-3BEBCEC18E69}"/>
+    <hyperlink ref="I4" r:id="rId5" xr:uid="{2C794336-F302-BF40-A6A8-F6430B6F5C8D}"/>
+    <hyperlink ref="I7" r:id="rId6" display="mailto:abcd1234@gmail.com" xr:uid="{1B7261E4-5300-5243-947E-BD3D9CAB8CE1}"/>
+    <hyperlink ref="I8" r:id="rId7" xr:uid="{DE7252F2-5BE8-CA4D-844C-508F345F69CD}"/>
+    <hyperlink ref="I9" r:id="rId8" xr:uid="{5495C219-2B02-C24B-848A-9BD92DACAC86}"/>
+    <hyperlink ref="I10" r:id="rId9" xr:uid="{D8835B11-7EE3-8245-AA5D-21C0D0311A7E}"/>
+    <hyperlink ref="I11" r:id="rId10" xr:uid="{83F21545-BDEF-DD48-9EFC-DA5824554D7D}"/>
+    <hyperlink ref="I12" r:id="rId11" xr:uid="{047DC6A4-66F6-F44C-9601-E12B7266B99C}"/>
+    <hyperlink ref="I13" r:id="rId12" xr:uid="{3B24F876-C054-B649-8B13-844E0898208C}"/>
+    <hyperlink ref="I14" r:id="rId13" xr:uid="{AE984405-5C38-B842-A2EC-FC6B17AAFD6C}"/>
+    <hyperlink ref="I15" r:id="rId14" display="abcd1234@gmail.com" xr:uid="{A9D42DA4-D802-0546-BA7B-31323FAA663B}"/>
+    <hyperlink ref="I16" r:id="rId15" display="abcd1234@gmail.com" xr:uid="{BBBD71DE-D4EF-F442-A4B2-BF9E5039F614}"/>
+    <hyperlink ref="I18" r:id="rId16" xr:uid="{FA25E08F-EB37-2B4C-B827-7B0F396795F4}"/>
+    <hyperlink ref="I19" r:id="rId17" xr:uid="{AE4E9F05-45A6-2342-9262-7AD7E240528D}"/>
+    <hyperlink ref="I1" r:id="rId18" xr:uid="{FC75257A-4F68-CC47-9B70-59276089ED63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>